<commit_message>
ajustes na filtragem dos arquivos, a fonte atualizou o filtro de SE para 28
</commit_message>
<xml_diff>
--- a/Data/g11.4.xlsx
+++ b/Data/g11.4.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,398 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1997</v>
+      </c>
+      <c r="B2" t="n">
+        <v>92534949.92261896</v>
+      </c>
+      <c r="C2" t="n">
+        <v>366107152.671737</v>
+      </c>
+      <c r="D2" t="n">
+        <v>603639380.3493997</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1998</v>
+      </c>
+      <c r="B3" t="n">
+        <v>73015573.13914414</v>
+      </c>
+      <c r="C3" t="n">
+        <v>144842530.7588122</v>
+      </c>
+      <c r="D3" t="n">
+        <v>694144378.455973</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1999</v>
+      </c>
+      <c r="B4" t="n">
+        <v>127533577.158244</v>
+      </c>
+      <c r="C4" t="n">
+        <v>94505985.09341794</v>
+      </c>
+      <c r="D4" t="n">
+        <v>641294859.4167044</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B5" t="n">
+        <v>117717354.2189644</v>
+      </c>
+      <c r="C5" t="n">
+        <v>85259607.93777138</v>
+      </c>
+      <c r="D5" t="n">
+        <v>765801677.4468803</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2001</v>
+      </c>
+      <c r="B6" t="n">
+        <v>193613346.4684302</v>
+      </c>
+      <c r="C6" t="n">
+        <v>55877348.80975366</v>
+      </c>
+      <c r="D6" t="n">
+        <v>870977414.0426997</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2002</v>
+      </c>
+      <c r="B7" t="n">
+        <v>179518694.6202532</v>
+      </c>
+      <c r="C7" t="n">
+        <v>902645898.4177215</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1078404236.075949</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2003</v>
+      </c>
+      <c r="B8" t="n">
+        <v>213193731.4856761</v>
+      </c>
+      <c r="C8" t="n">
+        <v>939701385.2872183</v>
+      </c>
+      <c r="D8" t="n">
+        <v>982696186.8700914</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2004</v>
+      </c>
+      <c r="B9" t="n">
+        <v>208492822.2225001</v>
+      </c>
+      <c r="C9" t="n">
+        <v>563701390.6239058</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1441165959.17788</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2005</v>
+      </c>
+      <c r="B10" t="n">
+        <v>153970883.8277984</v>
+      </c>
+      <c r="C10" t="n">
+        <v>511558922.3607715</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1783372958.611462</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2006</v>
+      </c>
+      <c r="B11" t="n">
+        <v>155630768.5524178</v>
+      </c>
+      <c r="C11" t="n">
+        <v>499792471.9320854</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1485635484.890729</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2007</v>
+      </c>
+      <c r="B12" t="n">
+        <v>77777261.54150286</v>
+      </c>
+      <c r="C12" t="n">
+        <v>621694178.2528318</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1540099115.439557</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2008</v>
+      </c>
+      <c r="B13" t="n">
+        <v>95870212.88534531</v>
+      </c>
+      <c r="C13" t="n">
+        <v>626151942.0153413</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1627125898.616248</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2009</v>
+      </c>
+      <c r="B14" t="n">
+        <v>96309323.66573989</v>
+      </c>
+      <c r="C14" t="n">
+        <v>657129917.6624393</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1657641692.098827</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B15" t="n">
+        <v>87563098.32237658</v>
+      </c>
+      <c r="C15" t="n">
+        <v>764624986.1314064</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1993118808.239646</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B16" t="n">
+        <v>82492684.56839997</v>
+      </c>
+      <c r="C16" t="n">
+        <v>785255510.4660183</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2207040594.443008</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B17" t="n">
+        <v>88806678.39962138</v>
+      </c>
+      <c r="C17" t="n">
+        <v>940284716.7317612</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2194751836.958079</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B18" t="n">
+        <v>231465122.7407945</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1068800287.814614</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2130230479.616107</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B19" t="n">
+        <v>266703630.3963684</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1086533080.168774</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2098966207.998798</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B20" t="n">
+        <v>231359992.4266163</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1015386024.421622</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1921532195.557813</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B21" t="n">
+        <v>206234994.1223276</v>
+      </c>
+      <c r="C21" t="n">
+        <v>924372641.5920178</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1882075451.245157</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B22" t="n">
+        <v>207922967.828885</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1097275594.047953</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1973059458.032405</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B23" t="n">
+        <v>216621050.4713161</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1051335925.556159</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1919784570.199054</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B24" t="n">
+        <v>247194582.859546</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1103886780.764249</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1881913482.410036</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B25" t="n">
+        <v>275570037.3710343</v>
+      </c>
+      <c r="C25" t="n">
+        <v>919798135.8751496</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1901960179.090258</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B26" t="n">
+        <v>325882679.0956431</v>
+      </c>
+      <c r="C26" t="n">
+        <v>958778950.811841</v>
+      </c>
+      <c r="D26" t="n">
+        <v>2110865612.403105</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B27" t="n">
+        <v>320859386.8942198</v>
+      </c>
+      <c r="C27" t="n">
+        <v>947217707.0477858</v>
+      </c>
+      <c r="D27" t="n">
+        <v>2255243528.627884</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B28" t="n">
+        <v>342904604.6797927</v>
+      </c>
+      <c r="C28" t="n">
+        <v>948722283.3989342</v>
+      </c>
+      <c r="D28" t="n">
+        <v>2616138411.594326</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B29" t="n">
+        <v>321365149.12</v>
+      </c>
+      <c r="C29" t="n">
+        <v>908436601.3599999</v>
+      </c>
+      <c r="D29" t="n">
+        <v>2884059718.07</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>